<commit_message>
update script for AF
update script for AF
</commit_message>
<xml_diff>
--- a/test_data/testdata.xlsx
+++ b/test_data/testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lephat/PycharmProjects/automation_mobile_pom/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351A154-89D1-ED47-BE0F-93A8074F4375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5240F645-8470-9944-95F4-B0E7A550349E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="10800" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="authentication" sheetId="3" r:id="rId1"/>
+    <sheet name="activity_feed" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -57,13 +58,25 @@
   </si>
   <si>
     <t>hmh5777</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generated by automation script: Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nam consectetur urna quis lacus volutpat, ut ornare nisi vestibulum. Vivamus malesuada porttitor scelerisque. Donec pellentesque cursus mi, id mollis metus tincidunt ut. In eu elementum dui, et commodo mi. Etiam ultrices diam in ante convallis porta. Phasellus vulputate sagittis pulvinar. Donec id velit facilisis, blandit dui nec, tempor velit. Morbi magna ante, condimentum ut diam semper, interdum consectetur urna. Nullam dignissim condimentum viverra. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +91,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,9 +120,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF31AFCC-E578-5648-8BBE-8C307E7417E4}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -470,4 +493,47 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AF4C4B-076D-7344-8B15-4198DB93DEC6}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="228" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>